<commit_message>
Avance xls y estamos con 10b
</commit_message>
<xml_diff>
--- a/Control_cumplimiento_consignas.xlsx
+++ b/Control_cumplimiento_consignas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniiaeedu-my.sharepoint.com/personal/mcancelas_mail_austral_edu_ar/Documents/MCD/IDW/dwa-lite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{108B7547-BB13-4D6E-AB80-9516708F6AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6B487B2-5D7D-44DA-AB5A-3163D27C767E}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{108B7547-BB13-4D6E-AB80-9516708F6AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{526487BA-8BCF-4E3F-AD02-D79E1AB663FD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0A0F3DF7-482F-4665-8943-D820821CD982}"/>
+    <workbookView minimized="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{0A0F3DF7-482F-4665-8943-D820821CD982}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -342,20 +342,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -364,14 +364,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -711,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3ECB10-D392-417F-A58E-F4E9037999B1}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,6 +713,7 @@
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
     <col min="3" max="7" width="11.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
@@ -735,69 +729,69 @@
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -811,233 +805,233 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>10</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>10</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>10</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>10</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>10</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>10</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>10</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>10</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>10</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>10</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
@@ -1051,103 +1045,103 @@
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>11</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>11</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>11</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>11</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>12</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>12</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>12</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
@@ -1161,7 +1155,7 @@
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="7">
         <v>13</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -1174,7 +1168,7 @@
       <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="A38" s="7">
         <v>13</v>
       </c>
       <c r="B38" s="10" t="s">
@@ -1187,7 +1181,7 @@
       <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="7">
         <v>13</v>
       </c>
       <c r="B39" s="10" t="s">
@@ -1200,7 +1194,7 @@
       <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="7">
         <v>13</v>
       </c>
       <c r="B40" s="10" t="s">
@@ -1213,7 +1207,7 @@
       <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="A41" s="7">
         <v>13</v>
       </c>
       <c r="B41" s="10" t="s">
@@ -1226,7 +1220,7 @@
       <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="A42" s="7">
         <v>13</v>
       </c>
       <c r="B42" s="10" t="s">
@@ -1239,7 +1233,7 @@
       <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="7">
         <v>13</v>
       </c>
       <c r="B43" s="10" t="s">
@@ -1252,142 +1246,142 @@
       <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+      <c r="A44" s="6">
         <v>14</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+      <c r="A45" s="6">
         <v>15</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
+      <c r="A46" s="6">
         <v>16</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
+      <c r="A47" s="6">
         <v>17</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+      <c r="A48" s="6">
         <v>18</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="A49" s="6">
         <v>19</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+      <c r="A50" s="6">
         <v>20</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+      <c r="A51" s="6">
         <v>21</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+      <c r="A52" s="6">
         <v>22</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+      <c r="A53" s="6">
         <v>23</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="5"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
@@ -1412,82 +1406,82 @@
       <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
+      <c r="A57" s="6">
         <v>1</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
     </row>
     <row r="58" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
+      <c r="A58" s="6">
         <v>2</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
+      <c r="A59" s="6">
         <v>3</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
     </row>
     <row r="60" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
+      <c r="A60" s="6">
         <v>4</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7">
+      <c r="A61" s="6">
         <v>5</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
+      <c r="A62" s="6">
         <v>6</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
     </row>
     <row r="65" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
@@ -1606,21 +1600,31 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B61:G61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="B58:G58"/>
     <mergeCell ref="B44:G44"/>
@@ -1629,6 +1633,16 @@
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="B49:G49"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A55:G55"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="B40:G40"/>
@@ -1640,31 +1654,11 @@
     <mergeCell ref="B32:G32"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="B62:G62"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:G5">
     <cfRule type="expression" dxfId="0" priority="2">

</xml_diff>